<commit_message>
Update SIRCREB y SIFERE
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\Importar RETPER SOS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF07C4A-D037-4F88-8C04-690ABF3197CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Control" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,41 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>CUIT</t>
+  </si>
+  <si>
+    <t>Controbuyente</t>
+  </si>
+  <si>
+    <t>Fila</t>
+  </si>
+  <si>
+    <t>RET 216</t>
+  </si>
+  <si>
+    <t>RET 217</t>
+  </si>
+  <si>
+    <t>RET 767</t>
+  </si>
+  <si>
+    <t>SIRCREB</t>
+  </si>
+  <si>
+    <t>SIFERE</t>
+  </si>
+  <si>
+    <t>CABA - AGIP</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +66,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +96,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +397,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add: mas opciones de RET PER
</commit_message>
<xml_diff>
--- a/Control.xlsx
+++ b/Control.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\Importar RETPER SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF07C4A-D037-4F88-8C04-690ABF3197CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB93C40-A2B8-444E-9C50-0ABBA4555403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CUIT</t>
   </si>
@@ -51,7 +62,25 @@
     <t>SIFERE</t>
   </si>
   <si>
-    <t>CABA - AGIP</t>
+    <t>PER 216</t>
+  </si>
+  <si>
+    <t>PER 217</t>
+  </si>
+  <si>
+    <t>PER 767</t>
+  </si>
+  <si>
+    <t>ARBA</t>
+  </si>
+  <si>
+    <t>CABA - AGIP RET</t>
+  </si>
+  <si>
+    <t>CABA - AGIP PER</t>
+  </si>
+  <si>
+    <t>SUSS</t>
   </si>
 </sst>
 </file>
@@ -398,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +438,7 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,13 +458,31 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>